<commit_message>
20180202T1240 Release Notes by ESPDInt integrated.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-Data_Structures-REGULATED-V02.00.01.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-Data_Structures-REGULATED-V02.00.01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="19440" windowHeight="6795"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="19440" windowHeight="6795" firstSheet="24" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -2743,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45799,7 +45799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y137"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -46847,8 +46849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7:V9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51566,7 +51568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -51872,8 +51874,8 @@
       <c r="A6" s="43"/>
       <c r="B6" s="42"/>
       <c r="C6" s="48"/>
-      <c r="D6" s="42" t="s">
-        <v>15</v>
+      <c r="D6" s="145" t="s">
+        <v>23</v>
       </c>
       <c r="E6" s="42"/>
       <c r="F6" s="42"/>
@@ -52018,8 +52020,8 @@
       <c r="A10" s="43"/>
       <c r="B10" s="42"/>
       <c r="C10" s="48"/>
-      <c r="D10" s="42" t="s">
-        <v>18</v>
+      <c r="D10" s="145" t="s">
+        <v>39</v>
       </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>

</xml_diff>